<commit_message>
Merging successful w/ formatting
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -480,17 +483,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>conduit1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>543+00</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
@@ -677,17 +680,17 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>conduit2</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>543+00</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="1" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
@@ -926,17 +929,17 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>conduit3</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="1" t="inlineStr">
         <is>
           <t>543+00</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="1" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
@@ -1071,17 +1074,17 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
         <is>
           <t>conduit4</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="1" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="1" t="inlineStr">
         <is>
           <t>554+90</t>
         </is>

</xml_diff>

<commit_message>
Merge + formatting fully done
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,84 +428,70 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="8" customWidth="1" min="8" max="8"/>
-    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Conduit Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Conduit</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Stationing Start</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Stationing End</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Cable Pull Numbers</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Pull #</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cable Size</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Express</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Diameter</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Weight</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Cross Sectional Area</t>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Free Air Space</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>conduit1</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>543+00</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="D2" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -513,21 +503,15 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1.73</v>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>60.42%</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="D3" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -539,21 +523,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G3" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.73</v>
-      </c>
     </row>
     <row r="4">
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="D4" s="2" t="n">
+        <v>15</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -565,21 +538,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.73</v>
-      </c>
     </row>
     <row r="5">
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="D5" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -591,21 +553,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1.73</v>
-      </c>
     </row>
     <row r="6">
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="D6" s="2" t="n">
+        <v>21</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -617,21 +568,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.73</v>
-      </c>
     </row>
     <row r="7">
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D7" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -643,21 +583,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="8">
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="D8" s="2" t="n">
+        <v>6</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -669,36 +598,25 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>conduit2</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 2</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>543+00</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="D9" s="2" t="n">
+        <v>7</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -710,21 +628,15 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G9" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.27</v>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>60.92%</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="D10" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -736,21 +648,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="11">
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="D11" s="2" t="n">
+        <v>9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -762,21 +663,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="12">
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="D12" s="2" t="n">
+        <v>11</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -788,21 +678,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G12" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="13">
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="D13" s="2" t="n">
+        <v>12</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -814,21 +693,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G13" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="14">
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="D14" s="2" t="n">
+        <v>13</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -840,21 +708,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I14" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="15">
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="D15" s="2" t="n">
+        <v>14</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -866,21 +723,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G15" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.767</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1.27</v>
-      </c>
     </row>
     <row r="16">
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="D16" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -892,21 +738,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>1.175</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1.08</v>
-      </c>
     </row>
     <row r="17">
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D17" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -918,36 +753,25 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G17" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>conduit3</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 3</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>543+00</t>
         </is>
       </c>
-      <c r="C18" s="1" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="D18" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -959,21 +783,15 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G18" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.77</v>
+      <c r="G18" s="2" t="inlineStr">
+        <is>
+          <t>86.38%</t>
+        </is>
       </c>
     </row>
     <row r="19">
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="D19" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -985,21 +803,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G19" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="20">
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="D20" s="2" t="n">
+        <v>17</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1011,21 +818,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G20" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="21">
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="D21" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1037,21 +833,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G21" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="22">
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="D22" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1063,36 +848,25 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G22" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>conduit4</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 4</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>553+00</t>
         </is>
       </c>
-      <c r="C23" s="1" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>554+90</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="D23" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1104,21 +878,15 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1.73</v>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>65.3%</t>
+        </is>
       </c>
     </row>
     <row r="24">
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="D24" s="2" t="n">
+        <v>18</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1130,21 +898,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G24" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1.73</v>
-      </c>
     </row>
     <row r="25">
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="D25" s="2" t="n">
+        <v>21</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1156,21 +913,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G25" t="n">
-        <v>1.485</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1.73</v>
-      </c>
     </row>
     <row r="26">
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D26" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1182,21 +928,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="27">
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="D27" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1208,21 +943,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G27" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="D28" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1234,21 +958,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G28" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="D29" s="2" t="n">
+        <v>17</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1260,21 +973,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G29" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="D30" s="2" t="n">
+        <v>19</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1286,21 +988,10 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="D31" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1312,30 +1003,25 @@
           <t>LOCAL</t>
         </is>
       </c>
-      <c r="G31" t="n">
-        <v>0.991</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0.77</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
     <mergeCell ref="C18:C22"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
+    <mergeCell ref="G18:G22"/>
     <mergeCell ref="C9:C17"/>
+    <mergeCell ref="A9:A17"/>
     <mergeCell ref="B9:B17"/>
-    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="G9:G17"/>
     <mergeCell ref="B23:B31"/>
     <mergeCell ref="C23:C31"/>
+    <mergeCell ref="G23:G31"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A23:A31"/>
     <mergeCell ref="C2:C8"/>
+    <mergeCell ref="G2:G8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Pdf output (not merged)
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -49,9 +49,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,7 +428,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -471,7 +474,663 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>543+00</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CABLE 2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>61.66%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3C#6</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CABLE 1</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 2</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>543+00</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>94.55%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 3</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>543+00</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>62.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 4</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>543+00</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G18" s="2" t="inlineStr">
+        <is>
+          <t>75.63%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>12C#14</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 5</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>554+90</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CABLE 2</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>74.54%</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CABLE 1</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 6</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>554+90</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>76.87%</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>7C#12</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="G18:G24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C17"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="G30:G35"/>
+    <mergeCell ref="G11:G17"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="B2:B8"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Centered output cells & starting local vs website
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,11 +491,11 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>7C#12</t>
+          <t>7C#14</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -505,215 +505,67 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>39.84%</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="n"/>
+          <t>10.91%</t>
+        </is>
+      </c>
     </row>
     <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 2</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>543+00</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
       <c r="D3" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>3C#6</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>21.82%</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Conduit 2</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>543+00</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>553+00</t>
-        </is>
-      </c>
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>12C#14</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>EXPRESS</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>35.84%</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="D5" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>12C#14</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="n"/>
-      <c r="G5" s="2" t="n"/>
-      <c r="H5" s="2" t="n"/>
-      <c r="I5" s="2" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Conduit 3</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>543+00</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>553+00</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>12C#14</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>EXPRESS</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>39.74%</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n"/>
-      <c r="I6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="D7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
           <t>7C#14</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n"/>
-      <c r="G7" s="2" t="n"/>
-      <c r="H7" s="2" t="n"/>
-      <c r="I7" s="2" t="n"/>
-    </row>
-    <row r="8">
-      <c r="D8" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>7C#14</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="n"/>
-      <c r="G8" s="2" t="n"/>
-      <c r="H8" s="2" t="n"/>
-      <c r="I8" s="2" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Conduit 4</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>543+00</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>553+00</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>2C#4</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>LOCAL</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>29.06%</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n"/>
-      <c r="I9" s="2" t="n"/>
-    </row>
-    <row r="10">
-      <c r="D10" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>2C#4</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="n"/>
-      <c r="G10" s="2" t="n"/>
-      <c r="H10" s="2" t="n"/>
-      <c r="I10" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B6:B8"/>
+  <mergeCells count="5">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Handles text stationing, duplicates tho
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,7 +428,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -500,41 +500,41 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>100+00</t>
+          <t>SWITCH-HTR-A</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>200+00</t>
+          <t>RELAY-RM-1</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>7C#14</t>
+          <t>STAR QUAD</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>LOCAL</t>
+          <t>EXPRESS</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>32.73%</t>
+          <t>38.88%</t>
         </is>
       </c>
       <c r="I2" s="2" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>24.05%</t>
+          <t>27.00%</t>
         </is>
       </c>
     </row>
@@ -543,11 +543,11 @@
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
       <c r="D3" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>7C#14</t>
+          <t>STAR QUAD</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -561,11 +561,11 @@
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>7C#14</t>
+          <t>STAR QUAD</t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -574,16 +574,1006 @@
       <c r="I4" s="2" t="n"/>
       <c r="J4" s="2" t="n"/>
     </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 2</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>32.73%</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>24.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 3</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>38.88%</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>27.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n"/>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 4</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>32.73%</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>24.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+      <c r="J12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 5</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>38.88%</t>
+        </is>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>27.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 6</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="inlineStr">
+        <is>
+          <t>32.73%</t>
+        </is>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J17" s="2" t="inlineStr">
+        <is>
+          <t>24.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="n"/>
+      <c r="I18" s="2" t="n"/>
+      <c r="J18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
+      <c r="I19" s="2" t="n"/>
+      <c r="J19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 7</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>38.88%</t>
+        </is>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J20" s="2" t="inlineStr">
+        <is>
+          <t>27.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n"/>
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n"/>
+      <c r="H21" s="2" t="n"/>
+      <c r="I21" s="2" t="n"/>
+      <c r="J21" s="2" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="2" t="n"/>
+      <c r="I22" s="2" t="n"/>
+      <c r="J22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 8</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>32.73%</t>
+        </is>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="2" t="inlineStr">
+        <is>
+          <t>24.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n"/>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="n"/>
+      <c r="H24" s="2" t="n"/>
+      <c r="I24" s="2" t="n"/>
+      <c r="J24" s="2" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n"/>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="n"/>
+      <c r="I25" s="2" t="n"/>
+      <c r="J25" s="2" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 9</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H26" s="2" t="inlineStr">
+        <is>
+          <t>38.88%</t>
+        </is>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" s="2" t="inlineStr">
+        <is>
+          <t>27.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="n"/>
+      <c r="I27" s="2" t="n"/>
+      <c r="J27" s="2" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n"/>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="n"/>
+      <c r="I28" s="2" t="n"/>
+      <c r="J28" s="2" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 10</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>32.73%</t>
+        </is>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J29" s="2" t="inlineStr">
+        <is>
+          <t>24.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n"/>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="n"/>
+      <c r="I30" s="2" t="n"/>
+      <c r="J30" s="2" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n"/>
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
+      <c r="H31" s="2" t="n"/>
+      <c r="I31" s="2" t="n"/>
+      <c r="J31" s="2" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 11</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>38.88%</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" s="2" t="inlineStr">
+        <is>
+          <t>27.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n"/>
+      <c r="B33" s="2" t="n"/>
+      <c r="C33" s="2" t="n"/>
+      <c r="D33" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="n"/>
+      <c r="G33" s="2" t="n"/>
+      <c r="H33" s="2" t="n"/>
+      <c r="I33" s="2" t="n"/>
+      <c r="J33" s="2" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n"/>
+      <c r="B34" s="2" t="n"/>
+      <c r="C34" s="2" t="n"/>
+      <c r="D34" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="n"/>
+      <c r="G34" s="2" t="n"/>
+      <c r="H34" s="2" t="n"/>
+      <c r="I34" s="2" t="n"/>
+      <c r="J34" s="2" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>Conduit 12</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>LOCAL</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t>32.73%</t>
+        </is>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J35" s="2" t="inlineStr">
+        <is>
+          <t>24.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n"/>
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
+      <c r="H36" s="2" t="n"/>
+      <c r="I36" s="2" t="n"/>
+      <c r="J36" s="2" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n"/>
+      <c r="B37" s="2" t="n"/>
+      <c r="C37" s="2" t="n"/>
+      <c r="D37" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="n"/>
+      <c r="G37" s="2" t="n"/>
+      <c r="H37" s="2" t="n"/>
+      <c r="I37" s="2" t="n"/>
+      <c r="J37" s="2" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="96">
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="G8:G10"/>
     <mergeCell ref="I2:I4"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="I17:I19"/>
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="C2:C4"/>
-    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="F20:F22"/>
     <mergeCell ref="F2:F4"/>
-    <mergeCell ref="J2:J4"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Output file with correct weight optimization
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,14 +428,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="24" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,24 +466,24 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Express</t>
+          <t>Express/Local</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Bundle Diameter</t>
+          <t>Bundle Diameter (in)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Bundle Weight</t>
+          <t>Bundle Weight (lb/mft)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Conduit 1</t>
+          <t>Bundle 1</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -497,11 +497,11 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>STAR QUAD</t>
+          <t>7C#14</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>2.7</v>
+        <v>30.71099999999998</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>2580</v>
+        <v>19.855</v>
       </c>
       <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
@@ -523,11 +523,11 @@
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
       <c r="D3" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>STAR QUAD</t>
+          <t>7C#14</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -541,11 +541,11 @@
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>STAR QUAD</t>
+          <t>7C#14</t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -555,40 +555,20 @@
       <c r="J4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Conduit 2</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>SWITCH-HTR-A</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>RELAY-RM-1</t>
-        </is>
-      </c>
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
       <c r="D5" s="2" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
           <t>7C#14</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>LOCAL</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>2.973</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>1485</v>
-      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
       <c r="I5" s="2" t="n"/>
       <c r="J5" s="2" t="n"/>
     </row>
@@ -597,7 +577,7 @@
       <c r="B6" s="2" t="n"/>
       <c r="C6" s="2" t="n"/>
       <c r="D6" s="2" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
@@ -615,7 +595,7 @@
       <c r="B7" s="2" t="n"/>
       <c r="C7" s="2" t="n"/>
       <c r="D7" s="2" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
@@ -628,24 +608,638 @@
       <c r="I7" s="2" t="n"/>
       <c r="J7" s="2" t="n"/>
     </row>
+    <row r="8">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n"/>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n"/>
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+      <c r="J12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="n"/>
+      <c r="H14" s="2" t="n"/>
+      <c r="I14" s="2" t="n"/>
+      <c r="J14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="n"/>
+      <c r="I18" s="2" t="n"/>
+      <c r="J18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
+      <c r="I19" s="2" t="n"/>
+      <c r="J19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="n"/>
+      <c r="I20" s="2" t="n"/>
+      <c r="J20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n"/>
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n"/>
+      <c r="H21" s="2" t="n"/>
+      <c r="I21" s="2" t="n"/>
+      <c r="J21" s="2" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="2" t="n"/>
+      <c r="I22" s="2" t="n"/>
+      <c r="J22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n"/>
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="n"/>
+      <c r="H23" s="2" t="n"/>
+      <c r="I23" s="2" t="n"/>
+      <c r="J23" s="2" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n"/>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="n"/>
+      <c r="H24" s="2" t="n"/>
+      <c r="I24" s="2" t="n"/>
+      <c r="J24" s="2" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n"/>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="n"/>
+      <c r="I25" s="2" t="n"/>
+      <c r="J25" s="2" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n"/>
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="n"/>
+      <c r="H26" s="2" t="n"/>
+      <c r="I26" s="2" t="n"/>
+      <c r="J26" s="2" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="n"/>
+      <c r="I27" s="2" t="n"/>
+      <c r="J27" s="2" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n"/>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="n"/>
+      <c r="I28" s="2" t="n"/>
+      <c r="J28" s="2" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n"/>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="2" t="n"/>
+      <c r="H29" s="2" t="n"/>
+      <c r="I29" s="2" t="n"/>
+      <c r="J29" s="2" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n"/>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="n"/>
+      <c r="I30" s="2" t="n"/>
+      <c r="J30" s="2" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n"/>
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
+      <c r="H31" s="2" t="n"/>
+      <c r="I31" s="2" t="n"/>
+      <c r="J31" s="2" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n"/>
+      <c r="B32" s="2" t="n"/>
+      <c r="C32" s="2" t="n"/>
+      <c r="D32" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="n"/>
+      <c r="G32" s="2" t="n"/>
+      <c r="H32" s="2" t="n"/>
+      <c r="I32" s="2" t="n"/>
+      <c r="J32" s="2" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n"/>
+      <c r="B33" s="2" t="n"/>
+      <c r="C33" s="2" t="n"/>
+      <c r="D33" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="n"/>
+      <c r="G33" s="2" t="n"/>
+      <c r="H33" s="2" t="n"/>
+      <c r="I33" s="2" t="n"/>
+      <c r="J33" s="2" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Bundle 2</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>6.300000000000001</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="I34" s="2" t="n"/>
+      <c r="J34" s="2" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n"/>
+      <c r="B35" s="2" t="n"/>
+      <c r="C35" s="2" t="n"/>
+      <c r="D35" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n"/>
+      <c r="G35" s="2" t="n"/>
+      <c r="H35" s="2" t="n"/>
+      <c r="I35" s="2" t="n"/>
+      <c r="J35" s="2" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n"/>
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
+      <c r="H36" s="2" t="n"/>
+      <c r="I36" s="2" t="n"/>
+      <c r="J36" s="2" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n"/>
+      <c r="B37" s="2" t="n"/>
+      <c r="C37" s="2" t="n"/>
+      <c r="D37" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="n"/>
+      <c r="G37" s="2" t="n"/>
+      <c r="H37" s="2" t="n"/>
+      <c r="I37" s="2" t="n"/>
+      <c r="J37" s="2" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n"/>
+      <c r="B38" s="2" t="n"/>
+      <c r="C38" s="2" t="n"/>
+      <c r="D38" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="n"/>
+      <c r="G38" s="2" t="n"/>
+      <c r="H38" s="2" t="n"/>
+      <c r="I38" s="2" t="n"/>
+      <c r="J38" s="2" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n"/>
+      <c r="B39" s="2" t="n"/>
+      <c r="C39" s="2" t="n"/>
+      <c r="D39" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="n"/>
+      <c r="G39" s="2" t="n"/>
+      <c r="H39" s="2" t="n"/>
+      <c r="I39" s="2" t="n"/>
+      <c r="J39" s="2" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n"/>
+      <c r="B40" s="2" t="n"/>
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>STAR QUAD</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="n"/>
+      <c r="G40" s="2" t="n"/>
+      <c r="H40" s="2" t="n"/>
+      <c r="I40" s="2" t="n"/>
+      <c r="J40" s="2" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="C34:C40"/>
+    <mergeCell ref="H34:H40"/>
+    <mergeCell ref="I34:I40"/>
+    <mergeCell ref="J34:J40"/>
+    <mergeCell ref="B2:B33"/>
+    <mergeCell ref="A2:A33"/>
+    <mergeCell ref="C2:C33"/>
+    <mergeCell ref="G2:G33"/>
+    <mergeCell ref="F2:F33"/>
+    <mergeCell ref="J2:J33"/>
+    <mergeCell ref="H2:H33"/>
+    <mergeCell ref="I2:I33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="G34:G40"/>
+    <mergeCell ref="F34:F40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Redid visualizer code to fit into current flow
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>30.71099999999998</v>
+        <v>29.81099999999998</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>19.855</v>
@@ -1059,9 +1059,21 @@
       <c r="J32" s="2" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n"/>
-      <c r="B33" s="2" t="n"/>
-      <c r="C33" s="2" t="n"/>
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Bundle 2</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>SWITCH-HTR-A</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>RELAY-RM-1</t>
+        </is>
+      </c>
       <c r="D33" s="2" t="n">
         <v>20</v>
       </c>
@@ -1070,28 +1082,24 @@
           <t>STAR QUAD</t>
         </is>
       </c>
-      <c r="F33" s="2" t="n"/>
-      <c r="G33" s="2" t="n"/>
-      <c r="H33" s="2" t="n"/>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>7.200000000000001</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>6.88</v>
+      </c>
       <c r="I33" s="2" t="n"/>
       <c r="J33" s="2" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Bundle 2</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>SWITCH-HTR-A</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="inlineStr">
-        <is>
-          <t>RELAY-RM-1</t>
-        </is>
-      </c>
+      <c r="A34" s="2" t="n"/>
+      <c r="B34" s="2" t="n"/>
+      <c r="C34" s="2" t="n"/>
       <c r="D34" s="2" t="n">
         <v>22</v>
       </c>
@@ -1100,17 +1108,9 @@
           <t>STAR QUAD</t>
         </is>
       </c>
-      <c r="F34" s="2" t="inlineStr">
-        <is>
-          <t>EXPRESS</t>
-        </is>
-      </c>
-      <c r="G34" s="2" t="n">
-        <v>6.300000000000001</v>
-      </c>
-      <c r="H34" s="2" t="n">
-        <v>6.02</v>
-      </c>
+      <c r="F34" s="2" t="n"/>
+      <c r="G34" s="2" t="n"/>
+      <c r="H34" s="2" t="n"/>
       <c r="I34" s="2" t="n"/>
       <c r="J34" s="2" t="n"/>
     </row>
@@ -1224,22 +1224,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="H34:H40"/>
-    <mergeCell ref="I34:I40"/>
-    <mergeCell ref="J34:J40"/>
-    <mergeCell ref="B2:B33"/>
-    <mergeCell ref="A2:A33"/>
-    <mergeCell ref="C2:C33"/>
-    <mergeCell ref="G2:G33"/>
-    <mergeCell ref="F2:F33"/>
-    <mergeCell ref="J2:J33"/>
-    <mergeCell ref="H2:H33"/>
-    <mergeCell ref="I2:I33"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="G34:G40"/>
-    <mergeCell ref="F34:F40"/>
+    <mergeCell ref="H33:H40"/>
+    <mergeCell ref="I33:I40"/>
+    <mergeCell ref="H2:H32"/>
+    <mergeCell ref="A2:A32"/>
+    <mergeCell ref="J33:J40"/>
+    <mergeCell ref="F2:F32"/>
+    <mergeCell ref="J2:J32"/>
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="F33:F40"/>
+    <mergeCell ref="C33:C40"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="G33:G40"/>
+    <mergeCell ref="B2:B32"/>
+    <mergeCell ref="I2:I32"/>
+    <mergeCell ref="C2:C32"/>
+    <mergeCell ref="G2:G32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bundle diameter calculations implemented
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,12 +488,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1000+00</t>
+          <t>543+00</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>1500+00</t>
+          <t>553+00</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
@@ -501,7 +501,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>CABLE 1</t>
+          <t>3C#9</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -510,13 +510,665 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1</v>
+        <v>5.885</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.5</v>
-      </c>
+        <v>14.22</v>
+      </c>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n"/>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n"/>
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+      <c r="J12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="n"/>
+      <c r="H14" s="2" t="n"/>
+      <c r="I14" s="2" t="n"/>
+      <c r="J14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="n"/>
+      <c r="I18" s="2" t="n"/>
+      <c r="J18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
+      <c r="I19" s="2" t="n"/>
+      <c r="J19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="n"/>
+      <c r="I20" s="2" t="n"/>
+      <c r="J20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n"/>
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n"/>
+      <c r="H21" s="2" t="n"/>
+      <c r="I21" s="2" t="n"/>
+      <c r="J21" s="2" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="2" t="n"/>
+      <c r="I22" s="2" t="n"/>
+      <c r="J22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n"/>
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="n"/>
+      <c r="H23" s="2" t="n"/>
+      <c r="I23" s="2" t="n"/>
+      <c r="J23" s="2" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n"/>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="n"/>
+      <c r="H24" s="2" t="n"/>
+      <c r="I24" s="2" t="n"/>
+      <c r="J24" s="2" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n"/>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="n"/>
+      <c r="I25" s="2" t="n"/>
+      <c r="J25" s="2" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n"/>
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="n"/>
+      <c r="H26" s="2" t="n"/>
+      <c r="I26" s="2" t="n"/>
+      <c r="J26" s="2" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="n"/>
+      <c r="I27" s="2" t="n"/>
+      <c r="J27" s="2" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n"/>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="n"/>
+      <c r="I28" s="2" t="n"/>
+      <c r="J28" s="2" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n"/>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="2" t="n"/>
+      <c r="H29" s="2" t="n"/>
+      <c r="I29" s="2" t="n"/>
+      <c r="J29" s="2" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n"/>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="n"/>
+      <c r="I30" s="2" t="n"/>
+      <c r="J30" s="2" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n"/>
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
+      <c r="H31" s="2" t="n"/>
+      <c r="I31" s="2" t="n"/>
+      <c r="J31" s="2" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n"/>
+      <c r="B32" s="2" t="n"/>
+      <c r="C32" s="2" t="n"/>
+      <c r="D32" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="n"/>
+      <c r="G32" s="2" t="n"/>
+      <c r="H32" s="2" t="n"/>
+      <c r="I32" s="2" t="n"/>
+      <c r="J32" s="2" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Bundle 2</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>543+00</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>553+00</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>2.685</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I33" s="2" t="n"/>
+      <c r="J33" s="2" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n"/>
+      <c r="B34" s="2" t="n"/>
+      <c r="C34" s="2" t="n"/>
+      <c r="D34" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="n"/>
+      <c r="G34" s="2" t="n"/>
+      <c r="H34" s="2" t="n"/>
+      <c r="I34" s="2" t="n"/>
+      <c r="J34" s="2" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n"/>
+      <c r="B35" s="2" t="n"/>
+      <c r="C35" s="2" t="n"/>
+      <c r="D35" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n"/>
+      <c r="G35" s="2" t="n"/>
+      <c r="H35" s="2" t="n"/>
+      <c r="I35" s="2" t="n"/>
+      <c r="J35" s="2" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n"/>
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>3C#9</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
+      <c r="H36" s="2" t="n"/>
+      <c r="I36" s="2" t="n"/>
+      <c r="J36" s="2" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="H2:H32"/>
+    <mergeCell ref="G33:G36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="A2:A32"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="F2:F32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="J2:J32"/>
+    <mergeCell ref="J33:J36"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="B2:B32"/>
+    <mergeCell ref="I2:I32"/>
+    <mergeCell ref="C2:C32"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="G2:G32"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Structure of two diameter
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,36 +509,64 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>2C#2</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>28.07%</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>20.62%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>2C#2</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>EXPRESS</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>38.6%</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>24.70%</t>
-        </is>
-      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="H2:H3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Duplicate Cable Drawing
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>7C#14</t>
+          <t>2C#2</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -510,43 +510,13 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>4.58</v>
+        <v>2.27</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>1.39</v>
-      </c>
-      <c r="I2" s="2" t="n"/>
-      <c r="J2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n"/>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>2C#2</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
+        <v>0.89</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="H2:H3"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Logic implemented but without relative coordinates
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,22 +501,52 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>EXPRESS</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
           <t>2C#2</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>EXPRESS</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>1.96</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>0.89</v>
-      </c>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="H2:H3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Two conductor cables included in diameter calculations but placement unoptimized
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.99</v>
+        <v>2.99</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>1.39</v>
+        <v>5.25</v>
       </c>
       <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
@@ -527,7 +527,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>2C#2</t>
+          <t>7C#14</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -536,16 +536,142 @@
       <c r="I3" s="2" t="n"/>
       <c r="J3" s="2" t="n"/>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>7C#14</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n"/>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>2C#2</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>2C#2</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I10"/>
+    <mergeCell ref="F2:F10"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="H2:H10"/>
+    <mergeCell ref="J2:J10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="G2:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Layout set, need to debug angling
</commit_message>
<xml_diff>
--- a/Output File.xlsx
+++ b/Output File.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,7 +513,7 @@
         <v>0.99</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>2.27</v>
+        <v>1.39</v>
       </c>
       <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
@@ -536,34 +536,16 @@
       <c r="I3" s="2" t="n"/>
       <c r="J3" s="2" t="n"/>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="n"/>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>2C#2</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>